<commit_message>
Updated the ER diagram, and added the queryLibTesting.sql file which will house all of the queries we will be using within the plugin. This file is purely for testing the database.
</commit_message>
<xml_diff>
--- a/CraftyProfessionsWorkbook.xlsx
+++ b/CraftyProfessionsWorkbook.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF44F55-442F-4359-83DE-D4D91231B38D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InitialExpEquation" sheetId="1" r:id="rId1"/>
+    <sheet name="AugmentList" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Base_Exp_Value">InitialExpEquation!$D$3</definedName>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Levels</t>
   </si>
@@ -43,12 +45,33 @@
   <si>
     <t>Cumulitive Exponential</t>
   </si>
+  <si>
+    <t>Profession Augments</t>
+  </si>
+  <si>
+    <t>Income Bonus</t>
+  </si>
+  <si>
+    <t>Token Bonus</t>
+  </si>
+  <si>
+    <t>Specialize Profession</t>
+  </si>
+  <si>
+    <t>Augment Name</t>
+  </si>
+  <si>
+    <t>Bonus Amount Minimum</t>
+  </si>
+  <si>
+    <t>Expierence Bonus</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +89,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -169,7 +215,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -197,6 +243,24 @@
     </xf>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2657,14 +2721,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:B51" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="A1:B51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A1:B51" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:B51" xr:uid="{00000000-0009-0000-0100-000004000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" name="Levels" dataDxfId="7"/>
-    <tableColumn id="2" name="Exp Amounts" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Levels" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Exp Amounts" dataDxfId="6">
       <calculatedColumnFormula>(Base_Exp_Value*A2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2673,14 +2737,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table424" displayName="Table424" ref="I1:J51" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
-  <autoFilter ref="I1:J51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table424" displayName="Table424" ref="I1:J51" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+  <autoFilter ref="I1:J51" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" name="Levels" dataDxfId="1"/>
-    <tableColumn id="2" name="Exp Amounts" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Levels" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Exp Amounts" dataDxfId="0">
       <calculatedColumnFormula>(Base_Exp_Value*I2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2950,11 +3014,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3823,4 +3887,131 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="15"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="10"/>
+    </row>
+    <row r="17" spans="12:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="12:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+    </row>
+    <row r="19" spans="12:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="12:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+    </row>
+    <row r="21" spans="12:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+    </row>
+    <row r="22" spans="12:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+    </row>
+    <row r="23" spans="12:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+    </row>
+    <row r="24" spans="12:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>